<commit_message>
Changes in handling of rows/columns
</commit_message>
<xml_diff>
--- a/FOIA SAR data/MEADS/2013 SAR MEADS Data Draw.xlsx
+++ b/FOIA SAR data/MEADS/2013 SAR MEADS Data Draw.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
-    <sheet name="CostSummary" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Funding Summary" sheetId="2" r:id="rId2"/>
     <sheet name="Annual Funding by Appropriation" sheetId="3" r:id="rId3"/>
     <sheet name="Unit Cost" sheetId="4" r:id="rId4"/>
     <sheet name="Unit Cost History" sheetId="5" r:id="rId5"/>
     <sheet name="Cost Variance" sheetId="6" r:id="rId6"/>
     <sheet name="Deliveries and Expenditures" sheetId="7" r:id="rId7"/>
-    <sheet name="Operating and Support CostTot" sheetId="8" r:id="rId8"/>
+    <sheet name="Operating and Support Cost" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1329,45 +1329,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1421,54 +1469,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1786,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1814,61 +1814,61 @@
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="131"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="97"/>
+      <c r="F2" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="99"/>
+      <c r="H2" s="100"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="132" t="s">
+      <c r="A3" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="129" t="s">
+      <c r="C3" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="131"/>
-      <c r="E3" s="129" t="s">
+      <c r="D3" s="100"/>
+      <c r="E3" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="133" t="s">
+      <c r="F3" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="133" t="s">
+      <c r="G3" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="133" t="s">
+      <c r="H3" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="134"/>
-      <c r="B4" s="134"/>
-      <c r="C4" s="135"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="137"/>
-      <c r="G4" s="137"/>
-      <c r="H4" s="137"/>
+      <c r="A4" s="103"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="138"/>
-      <c r="B5" s="138"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
-      <c r="H5" s="141"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="110"/>
+      <c r="G5" s="110"/>
+      <c r="H5" s="110"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -2180,61 +2180,61 @@
     </row>
     <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="126" t="s">
+      <c r="B19" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127"/>
-      <c r="E19" s="128"/>
-      <c r="F19" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="130"/>
-      <c r="H19" s="131"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="99"/>
+      <c r="H19" s="100"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="132" t="s">
+      <c r="A20" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="132" t="s">
+      <c r="B20" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="129" t="s">
+      <c r="C20" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="131"/>
-      <c r="E20" s="129" t="s">
+      <c r="D20" s="100"/>
+      <c r="E20" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="133" t="s">
+      <c r="F20" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="133" t="s">
+      <c r="G20" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="133" t="s">
+      <c r="H20" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="134"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="135"/>
-      <c r="D21" s="136"/>
-      <c r="E21" s="135"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="105"/>
+      <c r="E21" s="104"/>
+      <c r="F21" s="106"/>
+      <c r="G21" s="106"/>
+      <c r="H21" s="106"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="138"/>
-      <c r="B22" s="138"/>
-      <c r="C22" s="139"/>
-      <c r="D22" s="140"/>
-      <c r="E22" s="139"/>
-      <c r="F22" s="141"/>
-      <c r="G22" s="141"/>
-      <c r="H22" s="141"/>
+      <c r="A22" s="107"/>
+      <c r="B22" s="107"/>
+      <c r="C22" s="108"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="108"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
@@ -2606,61 +2606,61 @@
     </row>
     <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="126" t="s">
+      <c r="B41" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="127"/>
-      <c r="D41" s="127"/>
-      <c r="E41" s="128"/>
-      <c r="F41" s="129" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="130"/>
-      <c r="H41" s="131"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
+      <c r="E41" s="97"/>
+      <c r="F41" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="99"/>
+      <c r="H41" s="100"/>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="132" t="s">
+      <c r="A42" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B42" s="132" t="s">
+      <c r="B42" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="129" t="s">
+      <c r="C42" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="131"/>
-      <c r="E42" s="129" t="s">
+      <c r="D42" s="100"/>
+      <c r="E42" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="F42" s="133" t="s">
+      <c r="F42" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G42" s="133" t="s">
+      <c r="G42" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H42" s="133" t="s">
+      <c r="H42" s="102" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="134"/>
-      <c r="B43" s="134"/>
-      <c r="C43" s="135"/>
-      <c r="D43" s="136"/>
-      <c r="E43" s="135"/>
-      <c r="F43" s="137"/>
-      <c r="G43" s="137"/>
-      <c r="H43" s="137"/>
+      <c r="A43" s="103"/>
+      <c r="B43" s="103"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="106"/>
+      <c r="G43" s="106"/>
+      <c r="H43" s="106"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="138"/>
-      <c r="B44" s="138"/>
-      <c r="C44" s="139"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="139"/>
-      <c r="F44" s="141"/>
-      <c r="G44" s="141"/>
-      <c r="H44" s="141"/>
+      <c r="A44" s="107"/>
+      <c r="B44" s="107"/>
+      <c r="C44" s="108"/>
+      <c r="D44" s="109"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="110"/>
+      <c r="G44" s="110"/>
+      <c r="H44" s="110"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
@@ -3032,66 +3032,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="95"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="99" t="s">
+      <c r="D3" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="99" t="s">
+      <c r="E3" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="99" t="s">
+      <c r="F3" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="99" t="s">
+      <c r="G3" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="101" t="s">
+      <c r="H3" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="103" t="s">
+      <c r="I3" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="99" t="s">
+      <c r="J3" s="111" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="98"/>
-      <c r="B4" s="98"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="104"/>
-      <c r="J4" s="100"/>
+      <c r="A4" s="120"/>
+      <c r="B4" s="120"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="112"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -3333,67 +3333,67 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="107" t="s">
+      <c r="A13" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="107"/>
-      <c r="C13" s="107"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="95" t="s">
+      <c r="A14" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="95"/>
-      <c r="C14" s="95"/>
-      <c r="D14" s="95"/>
-      <c r="E14" s="95"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="118"/>
+      <c r="E14" s="118"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="105" t="s">
+      <c r="C15" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="99" t="s">
+      <c r="D15" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="99" t="s">
+      <c r="E15" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="99" t="s">
+      <c r="F15" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="99" t="s">
+      <c r="G15" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="101" t="s">
+      <c r="H15" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="103" t="s">
+      <c r="I15" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="99" t="s">
+      <c r="J15" s="111" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="98"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="100"/>
-      <c r="E16" s="100"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="100"/>
-      <c r="H16" s="102"/>
-      <c r="I16" s="104"/>
-      <c r="J16" s="100"/>
+      <c r="A16" s="120"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="114"/>
+      <c r="I16" s="116"/>
+      <c r="J16" s="112"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -3842,67 +3842,67 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="107" t="s">
+      <c r="A32" s="117" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="107"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="107"/>
-      <c r="E32" s="107"/>
+      <c r="B32" s="117"/>
+      <c r="C32" s="117"/>
+      <c r="D32" s="117"/>
+      <c r="E32" s="117"/>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="95" t="s">
+      <c r="A33" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="95"/>
-      <c r="C33" s="95"/>
-      <c r="D33" s="95"/>
-      <c r="E33" s="95"/>
+      <c r="B33" s="118"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="118"/>
+      <c r="E33" s="118"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="119" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="105" t="s">
+      <c r="C34" s="121" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="99" t="s">
+      <c r="D34" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="99" t="s">
+      <c r="E34" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="99" t="s">
+      <c r="F34" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="99" t="s">
+      <c r="G34" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="101" t="s">
+      <c r="H34" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="I34" s="103" t="s">
+      <c r="I34" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="99" t="s">
+      <c r="J34" s="111" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="98"/>
-      <c r="B35" s="98"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="100"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="100"/>
-      <c r="H35" s="102"/>
-      <c r="I35" s="104"/>
-      <c r="J35" s="100"/>
+      <c r="A35" s="120"/>
+      <c r="B35" s="120"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="112"/>
+      <c r="E35" s="112"/>
+      <c r="F35" s="112"/>
+      <c r="G35" s="112"/>
+      <c r="H35" s="114"/>
+      <c r="I35" s="116"/>
+      <c r="J35" s="112"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
@@ -4352,23 +4352,16 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A13:E13"/>
@@ -4378,16 +4371,23 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="F3:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4424,60 +4424,60 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="96" t="s">
+      <c r="C3" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="96" t="s">
+      <c r="D3" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="96" t="s">
+      <c r="E3" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="96" t="s">
+      <c r="F3" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="96" t="s">
+      <c r="G3" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="96" t="s">
+      <c r="H3" s="119" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="97"/>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="97"/>
+      <c r="A4" s="123"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="123"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
+      <c r="A5" s="123"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="98"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="98"/>
-      <c r="G6" s="98"/>
-      <c r="H6" s="98"/>
+      <c r="A6" s="120"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="120"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
+      <c r="G6" s="120"/>
+      <c r="H6" s="120"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -4766,11 +4766,11 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="108"/>
-      <c r="C19" s="108"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="124"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -4778,72 +4778,72 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109" t="s">
+      <c r="A20" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="109"/>
-      <c r="C20" s="109"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="96" t="s">
+      <c r="A21" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="96" t="s">
+      <c r="C21" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="96" t="s">
+      <c r="D21" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="96" t="s">
+      <c r="E21" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="96" t="s">
+      <c r="F21" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="96" t="s">
+      <c r="G21" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="96" t="s">
+      <c r="H21" s="119" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="97"/>
-      <c r="B22" s="97"/>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="97"/>
-      <c r="H22" s="97"/>
+      <c r="A22" s="123"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="123"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="97"/>
-      <c r="B23" s="97"/>
-      <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
+      <c r="E23" s="123"/>
+      <c r="F23" s="123"/>
+      <c r="G23" s="123"/>
+      <c r="H23" s="123"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="98"/>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
+      <c r="A24" s="120"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
@@ -5142,60 +5142,60 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="96" t="s">
+      <c r="B39" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="96" t="s">
+      <c r="C39" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="96" t="s">
+      <c r="D39" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="96" t="s">
+      <c r="E39" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="96" t="s">
+      <c r="F39" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="G39" s="96" t="s">
+      <c r="G39" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="96" t="s">
+      <c r="H39" s="119" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="97"/>
-      <c r="B40" s="97"/>
-      <c r="C40" s="97"/>
-      <c r="D40" s="97"/>
-      <c r="E40" s="97"/>
-      <c r="F40" s="97"/>
-      <c r="G40" s="97"/>
-      <c r="H40" s="97"/>
+      <c r="A40" s="123"/>
+      <c r="B40" s="123"/>
+      <c r="C40" s="123"/>
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="123"/>
+      <c r="H40" s="123"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="97"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="97"/>
-      <c r="D41" s="97"/>
-      <c r="E41" s="97"/>
-      <c r="F41" s="97"/>
-      <c r="G41" s="97"/>
-      <c r="H41" s="97"/>
+      <c r="A41" s="123"/>
+      <c r="B41" s="123"/>
+      <c r="C41" s="123"/>
+      <c r="D41" s="123"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="123"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="98"/>
-      <c r="B42" s="98"/>
-      <c r="C42" s="98"/>
-      <c r="D42" s="98"/>
-      <c r="E42" s="98"/>
-      <c r="F42" s="98"/>
-      <c r="G42" s="98"/>
-      <c r="H42" s="98"/>
+      <c r="A42" s="120"/>
+      <c r="B42" s="120"/>
+      <c r="C42" s="120"/>
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="120"/>
+      <c r="G42" s="120"/>
+      <c r="H42" s="120"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
@@ -5484,11 +5484,11 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="108" t="s">
+      <c r="A55" s="124" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="108"/>
-      <c r="C55" s="108"/>
+      <c r="B55" s="124"/>
+      <c r="C55" s="124"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -5496,72 +5496,72 @@
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="109" t="s">
+      <c r="A56" s="125" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="109"/>
-      <c r="C56" s="109"/>
-      <c r="D56" s="109"/>
-      <c r="E56" s="109"/>
-      <c r="F56" s="109"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
+      <c r="D56" s="125"/>
+      <c r="E56" s="125"/>
+      <c r="F56" s="125"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="96" t="s">
+      <c r="A57" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="96" t="s">
+      <c r="B57" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="96" t="s">
+      <c r="C57" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="96" t="s">
+      <c r="D57" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="96" t="s">
+      <c r="E57" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="F57" s="96" t="s">
+      <c r="F57" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="G57" s="96" t="s">
+      <c r="G57" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="H57" s="96" t="s">
+      <c r="H57" s="119" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="97"/>
-      <c r="B58" s="97"/>
-      <c r="C58" s="97"/>
-      <c r="D58" s="97"/>
-      <c r="E58" s="97"/>
-      <c r="F58" s="97"/>
-      <c r="G58" s="97"/>
-      <c r="H58" s="97"/>
+      <c r="A58" s="123"/>
+      <c r="B58" s="123"/>
+      <c r="C58" s="123"/>
+      <c r="D58" s="123"/>
+      <c r="E58" s="123"/>
+      <c r="F58" s="123"/>
+      <c r="G58" s="123"/>
+      <c r="H58" s="123"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="97"/>
-      <c r="B59" s="97"/>
-      <c r="C59" s="97"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="97"/>
-      <c r="F59" s="97"/>
-      <c r="G59" s="97"/>
-      <c r="H59" s="97"/>
+      <c r="A59" s="123"/>
+      <c r="B59" s="123"/>
+      <c r="C59" s="123"/>
+      <c r="D59" s="123"/>
+      <c r="E59" s="123"/>
+      <c r="F59" s="123"/>
+      <c r="G59" s="123"/>
+      <c r="H59" s="123"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="98"/>
-      <c r="B60" s="98"/>
-      <c r="C60" s="98"/>
-      <c r="D60" s="98"/>
-      <c r="E60" s="98"/>
-      <c r="F60" s="98"/>
-      <c r="G60" s="98"/>
-      <c r="H60" s="98"/>
+      <c r="A60" s="120"/>
+      <c r="B60" s="120"/>
+      <c r="C60" s="120"/>
+      <c r="D60" s="120"/>
+      <c r="E60" s="120"/>
+      <c r="F60" s="120"/>
+      <c r="G60" s="120"/>
+      <c r="H60" s="120"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -5860,60 +5860,60 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="96" t="s">
+      <c r="A75" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="96" t="s">
+      <c r="B75" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="96" t="s">
+      <c r="C75" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="96" t="s">
+      <c r="D75" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="E75" s="96" t="s">
+      <c r="E75" s="119" t="s">
         <v>51</v>
       </c>
-      <c r="F75" s="96" t="s">
+      <c r="F75" s="119" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="96" t="s">
+      <c r="G75" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="H75" s="96" t="s">
+      <c r="H75" s="119" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="97"/>
-      <c r="B76" s="97"/>
-      <c r="C76" s="97"/>
-      <c r="D76" s="97"/>
-      <c r="E76" s="97"/>
-      <c r="F76" s="97"/>
-      <c r="G76" s="97"/>
-      <c r="H76" s="97"/>
+      <c r="A76" s="123"/>
+      <c r="B76" s="123"/>
+      <c r="C76" s="123"/>
+      <c r="D76" s="123"/>
+      <c r="E76" s="123"/>
+      <c r="F76" s="123"/>
+      <c r="G76" s="123"/>
+      <c r="H76" s="123"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="97"/>
-      <c r="B77" s="97"/>
-      <c r="C77" s="97"/>
-      <c r="D77" s="97"/>
-      <c r="E77" s="97"/>
-      <c r="F77" s="97"/>
-      <c r="G77" s="97"/>
-      <c r="H77" s="97"/>
+      <c r="A77" s="123"/>
+      <c r="B77" s="123"/>
+      <c r="C77" s="123"/>
+      <c r="D77" s="123"/>
+      <c r="E77" s="123"/>
+      <c r="F77" s="123"/>
+      <c r="G77" s="123"/>
+      <c r="H77" s="123"/>
     </row>
     <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="98"/>
-      <c r="B78" s="98"/>
-      <c r="C78" s="98"/>
-      <c r="D78" s="98"/>
-      <c r="E78" s="98"/>
-      <c r="F78" s="98"/>
-      <c r="G78" s="98"/>
-      <c r="H78" s="98"/>
+      <c r="A78" s="120"/>
+      <c r="B78" s="120"/>
+      <c r="C78" s="120"/>
+      <c r="D78" s="120"/>
+      <c r="E78" s="120"/>
+      <c r="F78" s="120"/>
+      <c r="G78" s="120"/>
+      <c r="H78" s="120"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="51">
@@ -6524,60 +6524,60 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="96" t="s">
+      <c r="A105" s="119" t="s">
         <v>48</v>
       </c>
-      <c r="B105" s="96" t="s">
+      <c r="B105" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="C105" s="96" t="s">
+      <c r="C105" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="D105" s="96" t="s">
+      <c r="D105" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="E105" s="96" t="s">
+      <c r="E105" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="F105" s="96" t="s">
+      <c r="F105" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="G105" s="96" t="s">
+      <c r="G105" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="H105" s="96" t="s">
+      <c r="H105" s="119" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="97"/>
-      <c r="B106" s="97"/>
-      <c r="C106" s="97"/>
-      <c r="D106" s="97"/>
-      <c r="E106" s="97"/>
-      <c r="F106" s="97"/>
-      <c r="G106" s="97"/>
-      <c r="H106" s="97"/>
+      <c r="A106" s="123"/>
+      <c r="B106" s="123"/>
+      <c r="C106" s="123"/>
+      <c r="D106" s="123"/>
+      <c r="E106" s="123"/>
+      <c r="F106" s="123"/>
+      <c r="G106" s="123"/>
+      <c r="H106" s="123"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="97"/>
-      <c r="B107" s="97"/>
-      <c r="C107" s="97"/>
-      <c r="D107" s="97"/>
-      <c r="E107" s="97"/>
-      <c r="F107" s="97"/>
-      <c r="G107" s="97"/>
-      <c r="H107" s="97"/>
+      <c r="A107" s="123"/>
+      <c r="B107" s="123"/>
+      <c r="C107" s="123"/>
+      <c r="D107" s="123"/>
+      <c r="E107" s="123"/>
+      <c r="F107" s="123"/>
+      <c r="G107" s="123"/>
+      <c r="H107" s="123"/>
     </row>
     <row r="108" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="98"/>
-      <c r="B108" s="98"/>
-      <c r="C108" s="98"/>
-      <c r="D108" s="98"/>
-      <c r="E108" s="98"/>
-      <c r="F108" s="98"/>
-      <c r="G108" s="98"/>
-      <c r="H108" s="98"/>
+      <c r="A108" s="120"/>
+      <c r="B108" s="120"/>
+      <c r="C108" s="120"/>
+      <c r="D108" s="120"/>
+      <c r="E108" s="120"/>
+      <c r="F108" s="120"/>
+      <c r="G108" s="120"/>
+      <c r="H108" s="120"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="51">
@@ -7179,6 +7179,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="F105:F108"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="G75:G78"/>
+    <mergeCell ref="H75:H78"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="H3:H6"/>
     <mergeCell ref="A19:C19"/>
@@ -7195,42 +7231,6 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="F3:F6"/>
-    <mergeCell ref="G21:G24"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="H57:H60"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="G75:G78"/>
-    <mergeCell ref="H75:H78"/>
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="F105:F108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7258,11 +7258,11 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
-      <c r="B3" s="110" t="s">
+      <c r="B3" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="112"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="128"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
@@ -7373,11 +7373,11 @@
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53"/>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="112"/>
+      <c r="C14" s="127"/>
+      <c r="D14" s="128"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
@@ -7492,11 +7492,11 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="53"/>
-      <c r="B26" s="110" t="s">
+      <c r="B26" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="111"/>
-      <c r="D26" s="112"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="128"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
@@ -7607,11 +7607,11 @@
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="53"/>
-      <c r="B37" s="110" t="s">
+      <c r="B37" s="126" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="111"/>
-      <c r="D37" s="112"/>
+      <c r="C37" s="127"/>
+      <c r="D37" s="128"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="53" t="s">
@@ -7753,14 +7753,14 @@
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="112"/>
-      <c r="E2" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="112"/>
+      <c r="D2" s="128"/>
+      <c r="E2" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="128"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
@@ -7931,25 +7931,25 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="115" t="s">
+      <c r="B14" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="116"/>
-      <c r="I14" s="117"/>
-      <c r="J14" s="118" t="s">
+      <c r="C14" s="132"/>
+      <c r="D14" s="132"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="134" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="114"/>
+      <c r="A15" s="130"/>
       <c r="B15" s="63" t="s">
         <v>91</v>
       </c>
@@ -7974,7 +7974,7 @@
       <c r="I15" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="119"/>
+      <c r="J15" s="135"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -8014,25 +8014,25 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="115" t="s">
+      <c r="B19" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="117"/>
-      <c r="J19" s="118" t="s">
+      <c r="C19" s="132"/>
+      <c r="D19" s="132"/>
+      <c r="E19" s="132"/>
+      <c r="F19" s="132"/>
+      <c r="G19" s="132"/>
+      <c r="H19" s="132"/>
+      <c r="I19" s="133"/>
+      <c r="J19" s="134" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114"/>
+      <c r="A20" s="130"/>
       <c r="B20" s="63" t="s">
         <v>91</v>
       </c>
@@ -8057,7 +8057,7 @@
       <c r="I20" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="119"/>
+      <c r="J20" s="135"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -8099,14 +8099,14 @@
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
       <c r="B24" s="53"/>
-      <c r="C24" s="110" t="s">
+      <c r="C24" s="126" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="112"/>
-      <c r="E24" s="110" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="112"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="126" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="128"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
@@ -8277,25 +8277,25 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="113" t="s">
+      <c r="A36" s="129" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="116"/>
-      <c r="D36" s="116"/>
-      <c r="E36" s="116"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="117"/>
-      <c r="J36" s="118" t="s">
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="132"/>
+      <c r="G36" s="132"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="133"/>
+      <c r="J36" s="134" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="114"/>
+      <c r="A37" s="130"/>
       <c r="B37" s="65" t="s">
         <v>91</v>
       </c>
@@ -8320,7 +8320,7 @@
       <c r="I37" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="J37" s="119"/>
+      <c r="J37" s="135"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -8360,25 +8360,25 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="113" t="s">
+      <c r="A41" s="129" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="115" t="s">
+      <c r="B41" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="116"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="116"/>
-      <c r="I41" s="117"/>
-      <c r="J41" s="118" t="s">
+      <c r="C41" s="132"/>
+      <c r="D41" s="132"/>
+      <c r="E41" s="132"/>
+      <c r="F41" s="132"/>
+      <c r="G41" s="132"/>
+      <c r="H41" s="132"/>
+      <c r="I41" s="133"/>
+      <c r="J41" s="134" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="114"/>
+      <c r="A42" s="130"/>
       <c r="B42" s="65" t="s">
         <v>91</v>
       </c>
@@ -8403,7 +8403,7 @@
       <c r="I42" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="J42" s="119"/>
+      <c r="J42" s="135"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
@@ -8482,13 +8482,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="126" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="127"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="67"/>
@@ -8865,13 +8865,13 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="112"/>
+      <c r="B27" s="127"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="128"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="67"/>
@@ -9251,10 +9251,10 @@
       <c r="A52" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="122" t="s">
+      <c r="B52" s="138" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="123"/>
+      <c r="C52" s="139"/>
     </row>
     <row r="53" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="77" t="s">
@@ -9317,13 +9317,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="110" t="s">
+      <c r="A60" s="126" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="111"/>
-      <c r="C60" s="111"/>
-      <c r="D60" s="111"/>
-      <c r="E60" s="112"/>
+      <c r="B60" s="127"/>
+      <c r="C60" s="127"/>
+      <c r="D60" s="127"/>
+      <c r="E60" s="128"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="67"/>
@@ -9700,13 +9700,13 @@
     </row>
     <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="110" t="s">
+      <c r="A85" s="126" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="111"/>
-      <c r="C85" s="111"/>
-      <c r="D85" s="111"/>
-      <c r="E85" s="112"/>
+      <c r="B85" s="127"/>
+      <c r="C85" s="127"/>
+      <c r="D85" s="127"/>
+      <c r="E85" s="128"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="67"/>
@@ -10089,10 +10089,10 @@
       <c r="A110" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B110" s="122" t="s">
+      <c r="B110" s="138" t="s">
         <v>118</v>
       </c>
-      <c r="C110" s="123"/>
+      <c r="C110" s="139"/>
     </row>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="77" t="s">
@@ -10143,10 +10143,10 @@
       <c r="A116" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="120" t="s">
+      <c r="B116" s="136" t="s">
         <v>118</v>
       </c>
-      <c r="C116" s="121"/>
+      <c r="C116" s="137"/>
     </row>
     <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="82" t="s">
@@ -10354,12 +10354,12 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="110" t="s">
+      <c r="A7" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="112"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="127"/>
+      <c r="D7" s="128"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -10492,12 +10492,12 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="110" t="s">
+      <c r="A19" s="126" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="111"/>
-      <c r="C19" s="111"/>
-      <c r="D19" s="112"/>
+      <c r="B19" s="127"/>
+      <c r="C19" s="127"/>
+      <c r="D19" s="128"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -10568,8 +10568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10587,28 +10587,28 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="126" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="112"/>
+      <c r="C2" s="127"/>
+      <c r="D2" s="127"/>
+      <c r="E2" s="128"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="110" t="s">
+      <c r="C3" s="141"/>
+      <c r="D3" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="112"/>
+      <c r="E3" s="128"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="110" t="s">
+      <c r="B4" s="126" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="112"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="19" t="s">
         <v>149</v>
       </c>
@@ -10656,11 +10656,11 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="126" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="112"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="128"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
@@ -10763,28 +10763,28 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="110" t="s">
+      <c r="B20" s="126" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="112"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="128"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="140" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="125"/>
-      <c r="D21" s="110" t="s">
+      <c r="C21" s="141"/>
+      <c r="D21" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="112"/>
+      <c r="E21" s="128"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="110" t="s">
+      <c r="B22" s="126" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="112"/>
+      <c r="C22" s="128"/>
       <c r="D22" s="19" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
Added Section columns and useful filenames.
</commit_message>
<xml_diff>
--- a/FOIA SAR data/MEADS/2013 SAR MEADS Data Draw.xlsx
+++ b/FOIA SAR data/MEADS/2013 SAR MEADS Data Draw.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\R-scripts-and-data\FOIA SAR data\MEADS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\2007-01 PROFESSIONAL SERVICES\R scripts and data\FOIA SAR data\MEADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12180" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12270" firstSheet="3"/>
   </bookViews>
   <sheets>
     <sheet name="Cost Summary" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,7 +641,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="37">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -769,49 +769,9 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -1077,7 +1037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1089,13 +1049,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1112,28 +1072,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1142,7 +1102,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1151,10 +1111,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1166,10 +1126,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1184,13 +1144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1202,20 +1162,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1227,14 +1187,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1243,24 +1203,24 @@
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1275,58 +1235,58 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1353,47 +1313,35 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1401,34 +1349,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1449,26 +1385,53 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1563,23 +1526,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1615,23 +1561,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1784,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,261 +1735,293 @@
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="95" t="s">
+      <c r="A2" s="134"/>
+      <c r="B2" s="135" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="99"/>
-      <c r="H2" s="100"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="138" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="139"/>
+      <c r="H2" s="140"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="98" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="102" t="s">
+      <c r="F3" s="142" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="102" t="s">
+      <c r="G3" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="102" t="s">
+      <c r="H3" s="142" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="103"/>
-      <c r="B4" s="103"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
+      <c r="A4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8">
+        <v>4992.3</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4992.3</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3410.7</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5737</v>
+      </c>
+      <c r="G4" s="8">
+        <v>5737</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3897.7</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="107"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="16">
+        <v>17759.099999999999</v>
+      </c>
+      <c r="C5" s="16">
+        <v>17759.099999999999</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="16">
+        <v>5908.6</v>
+      </c>
+      <c r="F5" s="16">
+        <v>24158.400000000001</v>
+      </c>
+      <c r="G5" s="16">
+        <v>24158.400000000001</v>
+      </c>
+      <c r="H5" s="16">
+        <v>8718.6</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="8">
-        <v>4992.3</v>
-      </c>
-      <c r="C6" s="8">
-        <v>4992.3</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="8">
-        <v>3410.7</v>
-      </c>
-      <c r="F6" s="8">
-        <v>5737</v>
-      </c>
-      <c r="G6" s="8">
-        <v>5737</v>
-      </c>
-      <c r="H6" s="8">
-        <v>3897.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="16">
-        <v>17759.099999999999</v>
-      </c>
-      <c r="C7" s="16">
-        <v>17759.099999999999</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="16">
-        <v>5908.6</v>
-      </c>
-      <c r="F7" s="16">
-        <v>24158.400000000001</v>
-      </c>
-      <c r="G7" s="16">
-        <v>24158.400000000001</v>
-      </c>
-      <c r="H7" s="16">
-        <v>8718.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5397.5</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="9">
+        <v>7972.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5329.1</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="10">
+        <v>7889.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="9">
-        <v>5397.5</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="9">
-        <v>7972.8</v>
+        <v>11</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="16">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="16">
+        <v>83.2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="10">
-        <v>5329.1</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="10">
-        <v>7889.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="8">
+        <v>511.1</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="8">
+        <v>745.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="16">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="16">
-        <v>83.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="8">
+        <v>511.1</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="8">
+        <v>745.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="8">
-        <v>511.1</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="8">
-        <v>745.8</v>
+        <v>14</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="8">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="8">
-        <v>511.1</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>9</v>
+        <v>0</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
       </c>
       <c r="H12" s="8">
-        <v>745.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>9</v>
+      <c r="A13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="16">
+        <v>0</v>
+      </c>
+      <c r="C13" s="16">
+        <v>0</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>9</v>
@@ -2068,940 +2029,848 @@
       <c r="E13" s="16">
         <v>0</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>9</v>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="16">
+        <v>0</v>
       </c>
       <c r="H13" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>15</v>
+      <c r="A14" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="B14" s="8">
-        <v>0</v>
+        <v>22751.4</v>
       </c>
       <c r="C14" s="8">
-        <v>0</v>
+        <v>22751.4</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="E14" s="8">
-        <v>0</v>
+        <v>9319.2999999999993</v>
       </c>
       <c r="F14" s="8">
-        <v>0</v>
+        <v>29895.4</v>
       </c>
       <c r="G14" s="8">
-        <v>0</v>
+        <v>29895.4</v>
       </c>
       <c r="H14" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0</v>
-      </c>
-      <c r="C15" s="16">
-        <v>0</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="16">
-        <v>0</v>
-      </c>
-      <c r="F15" s="16">
-        <v>0</v>
-      </c>
-      <c r="G15" s="16">
-        <v>0</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12616.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="8">
-        <v>22751.4</v>
-      </c>
-      <c r="C16" s="8">
-        <v>22751.4</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="8">
-        <v>9319.2999999999993</v>
-      </c>
-      <c r="F16" s="8">
-        <v>29895.4</v>
-      </c>
-      <c r="G16" s="8">
-        <v>29895.4</v>
-      </c>
-      <c r="H16" s="8">
-        <v>12616.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="95" t="s">
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="95" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="97"/>
-      <c r="F19" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="G19" s="99"/>
-      <c r="H19" s="100"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="101" t="s">
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="99"/>
+      <c r="H17" s="100"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="101" t="s">
+      <c r="B18" s="101" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="98" t="s">
+      <c r="C18" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="100"/>
-      <c r="E20" s="98" t="s">
+      <c r="D18" s="100"/>
+      <c r="E18" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="102" t="s">
+      <c r="F18" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="G20" s="102" t="s">
+      <c r="G18" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H20" s="102" t="s">
+      <c r="H18" s="102" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="11">
+        <v>4531.3999999999996</v>
+      </c>
+      <c r="C19" s="11">
+        <v>4531.3999999999996</v>
+      </c>
+      <c r="D19" s="11">
+        <v>5211.1000000000004</v>
+      </c>
+      <c r="E19" s="11">
+        <v>2708.8</v>
+      </c>
+      <c r="F19" s="11">
+        <v>5255</v>
+      </c>
+      <c r="G19" s="11">
+        <v>5255</v>
+      </c>
+      <c r="H19" s="11">
+        <v>3112.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="17">
+        <v>11999.1</v>
+      </c>
+      <c r="C20" s="17">
+        <v>11999.1</v>
+      </c>
+      <c r="D20" s="17">
+        <v>13199</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0</v>
+      </c>
+      <c r="F20" s="17">
+        <v>16584.400000000001</v>
+      </c>
+      <c r="G20" s="17">
+        <v>16584.400000000001</v>
+      </c>
+      <c r="H20" s="17">
+        <v>0</v>
+      </c>
+    </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="103"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="107"/>
-      <c r="B22" s="107"/>
-      <c r="C22" s="108"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="108"/>
-      <c r="F22" s="110"/>
-      <c r="G22" s="110"/>
-      <c r="H22" s="110"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="11">
-        <v>4531.3999999999996</v>
-      </c>
-      <c r="C23" s="11">
-        <v>4531.3999999999996</v>
-      </c>
-      <c r="D23" s="11">
-        <v>5211.1000000000004</v>
-      </c>
-      <c r="E23" s="11">
-        <v>2708.8</v>
-      </c>
-      <c r="F23" s="11">
-        <v>5255</v>
-      </c>
-      <c r="G23" s="11">
-        <v>5255</v>
-      </c>
-      <c r="H23" s="11">
-        <v>3112.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="16">
+        <v>0</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B24" s="17">
-        <v>11999.1</v>
-      </c>
-      <c r="C24" s="17">
-        <v>11999.1</v>
-      </c>
-      <c r="D24" s="17">
-        <v>13199</v>
-      </c>
-      <c r="E24" s="17">
-        <v>0</v>
-      </c>
-      <c r="F24" s="17">
-        <v>16584.400000000001</v>
-      </c>
-      <c r="G24" s="17">
-        <v>16584.400000000001</v>
-      </c>
-      <c r="H24" s="17">
+        <v>12</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="8">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="16">
+        <v>0</v>
+      </c>
+      <c r="C28" s="16">
+        <v>0</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="16">
+        <v>0</v>
+      </c>
+      <c r="F28" s="16">
+        <v>0</v>
+      </c>
+      <c r="G28" s="16">
+        <v>0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="8">
+        <v>16530.5</v>
+      </c>
+      <c r="C29" s="8">
+        <v>16530.5</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="8">
+        <v>2708.8</v>
+      </c>
+      <c r="F29" s="8">
+        <v>21839.4</v>
+      </c>
+      <c r="G29" s="8">
+        <v>21839.4</v>
+      </c>
+      <c r="H29" s="8">
+        <v>3112.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="20">
+        <v>0</v>
+      </c>
+      <c r="C32" s="20">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="21">
+        <v>48</v>
+      </c>
+      <c r="C33" s="21">
+        <v>48</v>
+      </c>
+      <c r="D33" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="20">
+        <v>48</v>
+      </c>
+      <c r="C34">
+        <v>48</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="95" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="98" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="99"/>
+      <c r="H37" s="100"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="101" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="101" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="100"/>
+      <c r="E38" s="98" t="s">
+        <v>3</v>
+      </c>
+      <c r="F38" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="102" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="11">
+        <v>460.9</v>
+      </c>
+      <c r="C39" s="11">
+        <v>460.9</v>
+      </c>
+      <c r="D39" s="11">
+        <v>530</v>
+      </c>
+      <c r="E39" s="22">
+        <v>701.9</v>
+      </c>
+      <c r="F39" s="11">
+        <v>482</v>
+      </c>
+      <c r="G39" s="11">
+        <v>482</v>
+      </c>
+      <c r="H39" s="11">
+        <v>785.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="17">
+        <v>5760</v>
+      </c>
+      <c r="C40" s="17">
+        <v>5760</v>
+      </c>
+      <c r="D40" s="17">
+        <v>6336</v>
+      </c>
+      <c r="E40" s="17">
+        <v>5908.6</v>
+      </c>
+      <c r="F40" s="17">
+        <v>7574</v>
+      </c>
+      <c r="G40" s="17">
+        <v>7574</v>
+      </c>
+      <c r="H40" s="17">
+        <v>8718.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="B41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="9">
+        <v>0</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="9">
+        <v>7972.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="10">
-        <v>0</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="B42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="10">
+        <v>7889.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="16">
-        <v>0</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="B43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="16">
+        <v>0</v>
+      </c>
+      <c r="F43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="16">
+        <v>83.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="8">
-        <v>0</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="8">
-        <v>0</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="16">
-        <v>0</v>
-      </c>
-      <c r="F30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="8">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="8">
-        <v>0</v>
-      </c>
-      <c r="F31" s="8">
-        <v>0</v>
-      </c>
-      <c r="G31" s="8">
-        <v>0</v>
-      </c>
-      <c r="H31" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B32" s="16">
-        <v>0</v>
-      </c>
-      <c r="C32" s="16">
-        <v>0</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="16">
-        <v>0</v>
-      </c>
-      <c r="F32" s="16">
-        <v>0</v>
-      </c>
-      <c r="G32" s="16">
-        <v>0</v>
-      </c>
-      <c r="H32" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="8">
-        <v>16530.5</v>
-      </c>
-      <c r="C33" s="8">
-        <v>16530.5</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="8">
-        <v>2708.8</v>
-      </c>
-      <c r="F33" s="8">
-        <v>21839.4</v>
-      </c>
-      <c r="G33" s="8">
-        <v>21839.4</v>
-      </c>
-      <c r="H33" s="8">
-        <v>3112.4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="20">
-        <v>0</v>
-      </c>
-      <c r="C36" s="20">
-        <v>0</v>
-      </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="21">
-        <v>48</v>
-      </c>
-      <c r="C37" s="21">
-        <v>48</v>
-      </c>
-      <c r="D37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="20">
-        <v>48</v>
-      </c>
-      <c r="C38">
-        <v>48</v>
-      </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="C41" s="96"/>
-      <c r="D41" s="96"/>
-      <c r="E41" s="97"/>
-      <c r="F41" s="98" t="s">
-        <v>0</v>
-      </c>
-      <c r="G41" s="99"/>
-      <c r="H41" s="100"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="101" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="98" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42" s="100"/>
-      <c r="E42" s="98" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="102" t="s">
-        <v>4</v>
-      </c>
-      <c r="G42" s="102" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" s="102" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="103"/>
-      <c r="B43" s="103"/>
-      <c r="C43" s="104"/>
-      <c r="D43" s="105"/>
-      <c r="E43" s="104"/>
-      <c r="F43" s="106"/>
-      <c r="G43" s="106"/>
-      <c r="H43" s="106"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="107"/>
-      <c r="B44" s="107"/>
-      <c r="C44" s="108"/>
-      <c r="D44" s="109"/>
-      <c r="E44" s="108"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="110"/>
-      <c r="H44" s="110"/>
+      <c r="B44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="8">
+        <v>0</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="8">
+        <v>745.8</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="11">
-        <v>460.9</v>
-      </c>
-      <c r="C45" s="11">
-        <v>460.9</v>
-      </c>
-      <c r="D45" s="11">
-        <v>530</v>
-      </c>
-      <c r="E45" s="22">
-        <v>701.9</v>
-      </c>
-      <c r="F45" s="11">
-        <v>482</v>
-      </c>
-      <c r="G45" s="11">
-        <v>482</v>
-      </c>
-      <c r="H45" s="11">
-        <v>785.3</v>
+        <v>13</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="8">
+        <v>0</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="8">
+        <v>745.8</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B46" s="17">
-        <v>5760</v>
-      </c>
-      <c r="C46" s="17">
-        <v>5760</v>
-      </c>
-      <c r="D46" s="17">
-        <v>6336</v>
-      </c>
-      <c r="E46" s="17">
-        <v>5908.6</v>
-      </c>
-      <c r="F46" s="17">
-        <v>7574</v>
-      </c>
-      <c r="G46" s="17">
-        <v>7574</v>
-      </c>
-      <c r="H46" s="17">
-        <v>8718.6</v>
+        <v>14</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="16">
+        <v>0</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="9">
-        <v>0</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" s="9">
-        <v>7972.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="10">
-        <v>0</v>
-      </c>
-      <c r="F48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="10">
-        <v>7889.6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="16">
-        <v>0</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" s="16">
-        <v>83.2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="8">
-        <v>0</v>
-      </c>
-      <c r="F50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H50" s="8">
-        <v>745.8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="8">
-        <v>0</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H51" s="8">
-        <v>745.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="16">
-        <v>0</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H52" s="16">
+        <v>15</v>
+      </c>
+      <c r="B47" s="8">
+        <v>0</v>
+      </c>
+      <c r="C47" s="8">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="8">
+        <v>0</v>
+      </c>
+      <c r="F47" s="8">
+        <v>0</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0</v>
+      </c>
+      <c r="H47" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="16">
+        <v>0</v>
+      </c>
+      <c r="C48" s="16">
+        <v>0</v>
+      </c>
+      <c r="D48" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="16">
+        <v>0</v>
+      </c>
+      <c r="F48" s="16">
+        <v>0</v>
+      </c>
+      <c r="G48" s="16">
+        <v>0</v>
+      </c>
+      <c r="H48" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B49" s="8">
+        <v>6220.9</v>
+      </c>
+      <c r="C49" s="8">
+        <v>6220.9</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="8">
+        <v>6610.5</v>
+      </c>
+      <c r="F49" s="8">
+        <v>8056</v>
+      </c>
+      <c r="G49" s="8">
+        <v>8056</v>
+      </c>
+      <c r="H49" s="8">
+        <v>9503.9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" s="20">
+        <v>0</v>
+      </c>
+      <c r="C52" s="20">
+        <v>0</v>
+      </c>
+      <c r="D52">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B53" s="8">
-        <v>0</v>
-      </c>
-      <c r="C53" s="8">
-        <v>0</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="8">
-        <v>0</v>
-      </c>
-      <c r="F53" s="8">
-        <v>0</v>
-      </c>
-      <c r="G53" s="8">
-        <v>0</v>
-      </c>
-      <c r="H53" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B54" s="16">
-        <v>0</v>
-      </c>
-      <c r="C54" s="16">
-        <v>0</v>
-      </c>
-      <c r="D54" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="16">
-        <v>0</v>
-      </c>
-      <c r="F54" s="16">
-        <v>0</v>
-      </c>
-      <c r="G54" s="16">
-        <v>0</v>
-      </c>
-      <c r="H54" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="12" t="s">
+      <c r="A53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" s="21">
+        <v>1528</v>
+      </c>
+      <c r="C53" s="21">
+        <v>1528</v>
+      </c>
+      <c r="D53" s="7">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>17</v>
       </c>
-      <c r="B55" s="8">
-        <v>6220.9</v>
-      </c>
-      <c r="C55" s="8">
-        <v>6220.9</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="8">
-        <v>6610.5</v>
-      </c>
-      <c r="F55" s="8">
-        <v>8056</v>
-      </c>
-      <c r="G55" s="8">
-        <v>8056</v>
-      </c>
-      <c r="H55" s="8">
-        <v>9503.9</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="20">
-        <v>0</v>
-      </c>
-      <c r="C58" s="20">
-        <v>0</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B59" s="21">
+      <c r="B54" s="20">
         <v>1528</v>
       </c>
-      <c r="C59" s="21">
+      <c r="C54">
         <v>1528</v>
       </c>
-      <c r="D59" s="7">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="20">
-        <v>1528</v>
-      </c>
-      <c r="C60">
-        <v>1528</v>
-      </c>
-      <c r="D60">
+      <c r="D54">
         <v>1528</v>
       </c>
     </row>
@@ -3032,66 +2901,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="117" t="s">
+      <c r="A1" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="C3" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="111" t="s">
+      <c r="D3" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="111" t="s">
+      <c r="E3" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="111" t="s">
+      <c r="F3" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="111" t="s">
+      <c r="G3" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="113" t="s">
+      <c r="H3" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="111" t="s">
+      <c r="J3" s="103" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="120"/>
-      <c r="B4" s="120"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="114"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="112"/>
+      <c r="A4" s="110"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="108"/>
+      <c r="J4" s="104"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -3333,67 +3202,67 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="117"/>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="117"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
+      <c r="B14" s="114"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="114"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="119" t="s">
+      <c r="A15" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="119" t="s">
+      <c r="B15" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="121" t="s">
+      <c r="C15" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="111" t="s">
+      <c r="D15" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="111" t="s">
+      <c r="E15" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="111" t="s">
+      <c r="F15" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="111" t="s">
+      <c r="G15" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="113" t="s">
+      <c r="H15" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I15" s="115" t="s">
+      <c r="I15" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="111" t="s">
+      <c r="J15" s="103" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="120"/>
-      <c r="B16" s="120"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="112"/>
+      <c r="A16" s="110"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="112"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="104"/>
+      <c r="G16" s="104"/>
+      <c r="H16" s="106"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="104"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
@@ -3842,67 +3711,67 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="117" t="s">
+      <c r="A32" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="B32" s="117"/>
-      <c r="C32" s="117"/>
-      <c r="D32" s="117"/>
-      <c r="E32" s="117"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="113"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="113"/>
       <c r="K32" s="9"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="118" t="s">
+      <c r="A33" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="118"/>
-      <c r="C33" s="118"/>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="114"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="119" t="s">
+      <c r="B34" s="109" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="121" t="s">
+      <c r="C34" s="111" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="111" t="s">
+      <c r="D34" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="111" t="s">
+      <c r="E34" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="F34" s="111" t="s">
+      <c r="F34" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="111" t="s">
+      <c r="G34" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="113" t="s">
+      <c r="H34" s="105" t="s">
         <v>40</v>
       </c>
-      <c r="I34" s="115" t="s">
+      <c r="I34" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="J34" s="111" t="s">
+      <c r="J34" s="103" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="120"/>
-      <c r="B35" s="120"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="114"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="112"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="112"/>
+      <c r="D35" s="104"/>
+      <c r="E35" s="104"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="104"/>
+      <c r="H35" s="106"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="104"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
@@ -4352,16 +4221,23 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
     <mergeCell ref="A32:E32"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A13:E13"/>
@@ -4371,23 +4247,16 @@
     <mergeCell ref="D15:D16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J34:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4424,60 +4293,60 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="119" t="s">
+      <c r="B3" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="119" t="s">
+      <c r="D3" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="119" t="s">
+      <c r="E3" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="119" t="s">
+      <c r="F3" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="119" t="s">
+      <c r="G3" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H3" s="119" t="s">
+      <c r="H3" s="109" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="123"/>
-      <c r="B4" s="123"/>
-      <c r="C4" s="123"/>
-      <c r="D4" s="123"/>
-      <c r="E4" s="123"/>
-      <c r="F4" s="123"/>
-      <c r="G4" s="123"/>
-      <c r="H4" s="123"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="115"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="123"/>
-      <c r="B5" s="123"/>
-      <c r="C5" s="123"/>
-      <c r="D5" s="123"/>
-      <c r="E5" s="123"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="120"/>
-      <c r="B6" s="120"/>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -4766,11 +4635,11 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="116" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="124"/>
-      <c r="C19" s="124"/>
+      <c r="B19" s="116"/>
+      <c r="C19" s="116"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
@@ -4778,72 +4647,72 @@
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="125" t="s">
+      <c r="A20" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="117"/>
+      <c r="E20" s="117"/>
+      <c r="F20" s="117"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="119" t="s">
+      <c r="A21" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="119" t="s">
+      <c r="B21" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="119" t="s">
+      <c r="C21" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="119" t="s">
+      <c r="D21" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="119" t="s">
+      <c r="E21" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="119" t="s">
+      <c r="F21" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="119" t="s">
+      <c r="G21" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="119" t="s">
+      <c r="H21" s="109" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="123"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="123"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="115"/>
+      <c r="H23" s="115"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="120"/>
-      <c r="B24" s="120"/>
-      <c r="C24" s="120"/>
-      <c r="D24" s="120"/>
-      <c r="E24" s="120"/>
-      <c r="F24" s="120"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="120"/>
+      <c r="A24" s="110"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="110"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="110"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="110"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
@@ -5142,60 +5011,60 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="119" t="s">
+      <c r="A39" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="119" t="s">
+      <c r="B39" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="119" t="s">
+      <c r="C39" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="119" t="s">
+      <c r="D39" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="119" t="s">
+      <c r="E39" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="119" t="s">
+      <c r="F39" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="G39" s="119" t="s">
+      <c r="G39" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="119" t="s">
+      <c r="H39" s="109" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="123"/>
-      <c r="B40" s="123"/>
-      <c r="C40" s="123"/>
-      <c r="D40" s="123"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="123"/>
-      <c r="H40" s="123"/>
+      <c r="A40" s="115"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="115"/>
+      <c r="H40" s="115"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="123"/>
-      <c r="B41" s="123"/>
-      <c r="C41" s="123"/>
-      <c r="D41" s="123"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="123"/>
-      <c r="H41" s="123"/>
+      <c r="A41" s="115"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="115"/>
+      <c r="H41" s="115"/>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
-      <c r="B42" s="120"/>
-      <c r="C42" s="120"/>
-      <c r="D42" s="120"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="120"/>
-      <c r="G42" s="120"/>
-      <c r="H42" s="120"/>
+      <c r="A42" s="110"/>
+      <c r="B42" s="110"/>
+      <c r="C42" s="110"/>
+      <c r="D42" s="110"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="110"/>
+      <c r="G42" s="110"/>
+      <c r="H42" s="110"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
@@ -5484,11 +5353,11 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="124" t="s">
+      <c r="A55" s="116" t="s">
         <v>63</v>
       </c>
-      <c r="B55" s="124"/>
-      <c r="C55" s="124"/>
+      <c r="B55" s="116"/>
+      <c r="C55" s="116"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -5496,72 +5365,72 @@
       <c r="H55" s="4"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="125" t="s">
+      <c r="A56" s="117" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
-      <c r="D56" s="125"/>
-      <c r="E56" s="125"/>
-      <c r="F56" s="125"/>
+      <c r="B56" s="117"/>
+      <c r="C56" s="117"/>
+      <c r="D56" s="117"/>
+      <c r="E56" s="117"/>
+      <c r="F56" s="117"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="119" t="s">
+      <c r="A57" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="119" t="s">
+      <c r="B57" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="119" t="s">
+      <c r="C57" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="119" t="s">
+      <c r="D57" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="E57" s="119" t="s">
+      <c r="E57" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="F57" s="119" t="s">
+      <c r="F57" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="G57" s="119" t="s">
+      <c r="G57" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="H57" s="119" t="s">
+      <c r="H57" s="109" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="123"/>
-      <c r="B58" s="123"/>
-      <c r="C58" s="123"/>
-      <c r="D58" s="123"/>
-      <c r="E58" s="123"/>
-      <c r="F58" s="123"/>
-      <c r="G58" s="123"/>
-      <c r="H58" s="123"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="115"/>
+      <c r="C58" s="115"/>
+      <c r="D58" s="115"/>
+      <c r="E58" s="115"/>
+      <c r="F58" s="115"/>
+      <c r="G58" s="115"/>
+      <c r="H58" s="115"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="123"/>
-      <c r="B59" s="123"/>
-      <c r="C59" s="123"/>
-      <c r="D59" s="123"/>
-      <c r="E59" s="123"/>
-      <c r="F59" s="123"/>
-      <c r="G59" s="123"/>
-      <c r="H59" s="123"/>
+      <c r="A59" s="115"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="115"/>
+      <c r="G59" s="115"/>
+      <c r="H59" s="115"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="120"/>
-      <c r="B60" s="120"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="120"/>
-      <c r="E60" s="120"/>
-      <c r="F60" s="120"/>
-      <c r="G60" s="120"/>
-      <c r="H60" s="120"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="110"/>
+      <c r="C60" s="110"/>
+      <c r="D60" s="110"/>
+      <c r="E60" s="110"/>
+      <c r="F60" s="110"/>
+      <c r="G60" s="110"/>
+      <c r="H60" s="110"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
@@ -5860,60 +5729,60 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="119" t="s">
+      <c r="A75" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="119" t="s">
+      <c r="B75" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C75" s="119" t="s">
+      <c r="C75" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="119" t="s">
+      <c r="D75" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="E75" s="119" t="s">
+      <c r="E75" s="109" t="s">
         <v>51</v>
       </c>
-      <c r="F75" s="119" t="s">
+      <c r="F75" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="119" t="s">
+      <c r="G75" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="H75" s="119" t="s">
+      <c r="H75" s="109" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="123"/>
-      <c r="B76" s="123"/>
-      <c r="C76" s="123"/>
-      <c r="D76" s="123"/>
-      <c r="E76" s="123"/>
-      <c r="F76" s="123"/>
-      <c r="G76" s="123"/>
-      <c r="H76" s="123"/>
+      <c r="A76" s="115"/>
+      <c r="B76" s="115"/>
+      <c r="C76" s="115"/>
+      <c r="D76" s="115"/>
+      <c r="E76" s="115"/>
+      <c r="F76" s="115"/>
+      <c r="G76" s="115"/>
+      <c r="H76" s="115"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="123"/>
-      <c r="B77" s="123"/>
-      <c r="C77" s="123"/>
-      <c r="D77" s="123"/>
-      <c r="E77" s="123"/>
-      <c r="F77" s="123"/>
-      <c r="G77" s="123"/>
-      <c r="H77" s="123"/>
+      <c r="A77" s="115"/>
+      <c r="B77" s="115"/>
+      <c r="C77" s="115"/>
+      <c r="D77" s="115"/>
+      <c r="E77" s="115"/>
+      <c r="F77" s="115"/>
+      <c r="G77" s="115"/>
+      <c r="H77" s="115"/>
     </row>
     <row r="78" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="120"/>
-      <c r="B78" s="120"/>
-      <c r="C78" s="120"/>
-      <c r="D78" s="120"/>
-      <c r="E78" s="120"/>
-      <c r="F78" s="120"/>
-      <c r="G78" s="120"/>
-      <c r="H78" s="120"/>
+      <c r="A78" s="110"/>
+      <c r="B78" s="110"/>
+      <c r="C78" s="110"/>
+      <c r="D78" s="110"/>
+      <c r="E78" s="110"/>
+      <c r="F78" s="110"/>
+      <c r="G78" s="110"/>
+      <c r="H78" s="110"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="51">
@@ -6524,60 +6393,60 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="119" t="s">
+      <c r="A105" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="B105" s="119" t="s">
+      <c r="B105" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="C105" s="119" t="s">
+      <c r="C105" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="D105" s="119" t="s">
+      <c r="D105" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="E105" s="119" t="s">
+      <c r="E105" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="F105" s="119" t="s">
+      <c r="F105" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="G105" s="119" t="s">
+      <c r="G105" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="H105" s="119" t="s">
+      <c r="H105" s="109" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="123"/>
-      <c r="B106" s="123"/>
-      <c r="C106" s="123"/>
-      <c r="D106" s="123"/>
-      <c r="E106" s="123"/>
-      <c r="F106" s="123"/>
-      <c r="G106" s="123"/>
-      <c r="H106" s="123"/>
+      <c r="A106" s="115"/>
+      <c r="B106" s="115"/>
+      <c r="C106" s="115"/>
+      <c r="D106" s="115"/>
+      <c r="E106" s="115"/>
+      <c r="F106" s="115"/>
+      <c r="G106" s="115"/>
+      <c r="H106" s="115"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="123"/>
-      <c r="B107" s="123"/>
-      <c r="C107" s="123"/>
-      <c r="D107" s="123"/>
-      <c r="E107" s="123"/>
-      <c r="F107" s="123"/>
-      <c r="G107" s="123"/>
-      <c r="H107" s="123"/>
+      <c r="A107" s="115"/>
+      <c r="B107" s="115"/>
+      <c r="C107" s="115"/>
+      <c r="D107" s="115"/>
+      <c r="E107" s="115"/>
+      <c r="F107" s="115"/>
+      <c r="G107" s="115"/>
+      <c r="H107" s="115"/>
     </row>
     <row r="108" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="120"/>
-      <c r="B108" s="120"/>
-      <c r="C108" s="120"/>
-      <c r="D108" s="120"/>
-      <c r="E108" s="120"/>
-      <c r="F108" s="120"/>
-      <c r="G108" s="120"/>
-      <c r="H108" s="120"/>
+      <c r="A108" s="110"/>
+      <c r="B108" s="110"/>
+      <c r="C108" s="110"/>
+      <c r="D108" s="110"/>
+      <c r="E108" s="110"/>
+      <c r="F108" s="110"/>
+      <c r="G108" s="110"/>
+      <c r="H108" s="110"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="51">
@@ -7179,42 +7048,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="G105:G108"/>
-    <mergeCell ref="H105:H108"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="C105:C108"/>
-    <mergeCell ref="D105:D108"/>
-    <mergeCell ref="E105:E108"/>
-    <mergeCell ref="F105:F108"/>
-    <mergeCell ref="G57:G60"/>
-    <mergeCell ref="H57:H60"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="C75:C78"/>
-    <mergeCell ref="D75:D78"/>
-    <mergeCell ref="E75:E78"/>
-    <mergeCell ref="F75:F78"/>
-    <mergeCell ref="G75:G78"/>
-    <mergeCell ref="H75:H78"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A56:F56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="C57:C60"/>
-    <mergeCell ref="D57:D60"/>
-    <mergeCell ref="E57:E60"/>
-    <mergeCell ref="F57:F60"/>
-    <mergeCell ref="G21:G24"/>
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="D39:D42"/>
-    <mergeCell ref="E39:E42"/>
-    <mergeCell ref="F39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
     <mergeCell ref="G3:G6"/>
     <mergeCell ref="H3:H6"/>
     <mergeCell ref="A19:C19"/>
@@ -7231,6 +7064,42 @@
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="E3:E6"/>
     <mergeCell ref="F3:F6"/>
+    <mergeCell ref="G21:G24"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:D42"/>
+    <mergeCell ref="E39:E42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A56:F56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="D57:D60"/>
+    <mergeCell ref="E57:E60"/>
+    <mergeCell ref="F57:F60"/>
+    <mergeCell ref="G57:G60"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="C75:C78"/>
+    <mergeCell ref="D75:D78"/>
+    <mergeCell ref="E75:E78"/>
+    <mergeCell ref="F75:F78"/>
+    <mergeCell ref="G75:G78"/>
+    <mergeCell ref="H75:H78"/>
+    <mergeCell ref="G105:G108"/>
+    <mergeCell ref="H105:H108"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="C105:C108"/>
+    <mergeCell ref="D105:D108"/>
+    <mergeCell ref="E105:E108"/>
+    <mergeCell ref="F105:F108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7258,11 +7127,11 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="128"/>
+      <c r="C3" s="119"/>
+      <c r="D3" s="120"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="53" t="s">
@@ -7373,11 +7242,11 @@
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53"/>
-      <c r="B14" s="126" t="s">
+      <c r="B14" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="128"/>
+      <c r="C14" s="119"/>
+      <c r="D14" s="120"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="53" t="s">
@@ -7492,11 +7361,11 @@
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="53"/>
-      <c r="B26" s="126" t="s">
+      <c r="B26" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="128"/>
+      <c r="C26" s="119"/>
+      <c r="D26" s="120"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="53" t="s">
@@ -7607,11 +7476,11 @@
     <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="53"/>
-      <c r="B37" s="126" t="s">
+      <c r="B37" s="118" t="s">
         <v>68</v>
       </c>
-      <c r="C37" s="127"/>
-      <c r="D37" s="128"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="120"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="53" t="s">
@@ -7753,14 +7622,14 @@
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="53"/>
       <c r="B2" s="53"/>
-      <c r="C2" s="126" t="s">
+      <c r="C2" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="128"/>
-      <c r="E2" s="126" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="128"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="120"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="53"/>
@@ -7931,25 +7800,25 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="129" t="s">
+      <c r="A14" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="131" t="s">
+      <c r="B14" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="C14" s="132"/>
-      <c r="D14" s="132"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="133"/>
-      <c r="J14" s="134" t="s">
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125"/>
+      <c r="J14" s="126" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="130"/>
+      <c r="A15" s="122"/>
       <c r="B15" s="63" t="s">
         <v>91</v>
       </c>
@@ -7974,7 +7843,7 @@
       <c r="I15" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="J15" s="135"/>
+      <c r="J15" s="127"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -8014,25 +7883,25 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="129" t="s">
+      <c r="A19" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="131" t="s">
+      <c r="B19" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="C19" s="132"/>
-      <c r="D19" s="132"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
-      <c r="G19" s="132"/>
-      <c r="H19" s="132"/>
-      <c r="I19" s="133"/>
-      <c r="J19" s="134" t="s">
+      <c r="C19" s="124"/>
+      <c r="D19" s="124"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="124"/>
+      <c r="H19" s="124"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="126" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="130"/>
+      <c r="A20" s="122"/>
       <c r="B20" s="63" t="s">
         <v>91</v>
       </c>
@@ -8057,7 +7926,7 @@
       <c r="I20" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="135"/>
+      <c r="J20" s="127"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
@@ -8099,14 +7968,14 @@
     <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="53"/>
       <c r="B24" s="53"/>
-      <c r="C24" s="126" t="s">
+      <c r="C24" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="128"/>
-      <c r="E24" s="126" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="128"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="118" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="120"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="53"/>
@@ -8277,25 +8146,25 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="129" t="s">
+      <c r="A36" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="B36" s="131" t="s">
+      <c r="B36" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="C36" s="132"/>
-      <c r="D36" s="132"/>
-      <c r="E36" s="132"/>
-      <c r="F36" s="132"/>
-      <c r="G36" s="132"/>
-      <c r="H36" s="132"/>
-      <c r="I36" s="133"/>
-      <c r="J36" s="134" t="s">
+      <c r="C36" s="124"/>
+      <c r="D36" s="124"/>
+      <c r="E36" s="124"/>
+      <c r="F36" s="124"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="124"/>
+      <c r="I36" s="125"/>
+      <c r="J36" s="126" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="130"/>
+      <c r="A37" s="122"/>
       <c r="B37" s="65" t="s">
         <v>91</v>
       </c>
@@ -8320,7 +8189,7 @@
       <c r="I37" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="J37" s="135"/>
+      <c r="J37" s="127"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
@@ -8360,25 +8229,25 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="129" t="s">
+      <c r="A41" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="B41" s="131" t="s">
+      <c r="B41" s="123" t="s">
         <v>89</v>
       </c>
-      <c r="C41" s="132"/>
-      <c r="D41" s="132"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="132"/>
-      <c r="G41" s="132"/>
-      <c r="H41" s="132"/>
-      <c r="I41" s="133"/>
-      <c r="J41" s="134" t="s">
+      <c r="C41" s="124"/>
+      <c r="D41" s="124"/>
+      <c r="E41" s="124"/>
+      <c r="F41" s="124"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="124"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="126" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="130"/>
+      <c r="A42" s="122"/>
       <c r="B42" s="65" t="s">
         <v>91</v>
       </c>
@@ -8403,7 +8272,7 @@
       <c r="I42" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="J42" s="135"/>
+      <c r="J42" s="127"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
@@ -8482,13 +8351,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="127"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="128"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="120"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="67"/>
@@ -8865,13 +8734,13 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="126" t="s">
+      <c r="A27" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="B27" s="127"/>
-      <c r="C27" s="127"/>
-      <c r="D27" s="127"/>
-      <c r="E27" s="128"/>
+      <c r="B27" s="119"/>
+      <c r="C27" s="119"/>
+      <c r="D27" s="119"/>
+      <c r="E27" s="120"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="67"/>
@@ -9251,10 +9120,10 @@
       <c r="A52" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="138" t="s">
+      <c r="B52" s="130" t="s">
         <v>118</v>
       </c>
-      <c r="C52" s="139"/>
+      <c r="C52" s="131"/>
     </row>
     <row r="53" spans="1:5" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="77" t="s">
@@ -9317,13 +9186,13 @@
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="126" t="s">
+      <c r="A60" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="127"/>
-      <c r="C60" s="127"/>
-      <c r="D60" s="127"/>
-      <c r="E60" s="128"/>
+      <c r="B60" s="119"/>
+      <c r="C60" s="119"/>
+      <c r="D60" s="119"/>
+      <c r="E60" s="120"/>
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="67"/>
@@ -9700,13 +9569,13 @@
     </row>
     <row r="84" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="85" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="126" t="s">
+      <c r="A85" s="118" t="s">
         <v>117</v>
       </c>
-      <c r="B85" s="127"/>
-      <c r="C85" s="127"/>
-      <c r="D85" s="127"/>
-      <c r="E85" s="128"/>
+      <c r="B85" s="119"/>
+      <c r="C85" s="119"/>
+      <c r="D85" s="119"/>
+      <c r="E85" s="120"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="67"/>
@@ -10089,10 +9958,10 @@
       <c r="A110" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B110" s="138" t="s">
+      <c r="B110" s="130" t="s">
         <v>118</v>
       </c>
-      <c r="C110" s="139"/>
+      <c r="C110" s="131"/>
     </row>
     <row r="111" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A111" s="77" t="s">
@@ -10143,10 +10012,10 @@
       <c r="A116" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B116" s="136" t="s">
+      <c r="B116" s="128" t="s">
         <v>118</v>
       </c>
-      <c r="C116" s="137"/>
+      <c r="C116" s="129"/>
     </row>
     <row r="117" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A117" s="82" t="s">
@@ -10354,12 +10223,12 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="126" t="s">
+      <c r="A7" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="127"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="128"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="120"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -10492,12 +10361,12 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="126" t="s">
+      <c r="A19" s="118" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127"/>
-      <c r="D19" s="128"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="119"/>
+      <c r="D19" s="120"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -10568,7 +10437,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -10587,28 +10456,28 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="128"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="120"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="132" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="126" t="s">
+      <c r="C3" s="133"/>
+      <c r="D3" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="128"/>
+      <c r="E3" s="120"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="118" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="128"/>
+      <c r="C4" s="120"/>
       <c r="D4" s="19" t="s">
         <v>149</v>
       </c>
@@ -10656,11 +10525,11 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="126" t="s">
+      <c r="A9" s="118" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="127"/>
-      <c r="C9" s="128"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="120"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="53" t="s">
@@ -10763,28 +10632,28 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="118" t="s">
         <v>151</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="128"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="119"/>
+      <c r="E20" s="120"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="140" t="s">
+      <c r="B21" s="132" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="141"/>
-      <c r="D21" s="126" t="s">
+      <c r="C21" s="133"/>
+      <c r="D21" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="128"/>
+      <c r="E21" s="120"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="126" t="s">
+      <c r="B22" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="128"/>
+      <c r="C22" s="120"/>
       <c r="D22" s="19" t="s">
         <v>149</v>
       </c>

</xml_diff>